<commit_message>
Fix longest_horizontal_row calculation in vertical orientation
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/commands_in_metatab.xlsx
+++ b/flattentool/tests/fixtures/xlsx/commands_in_metatab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t xml:space="preserve">HeaderRows 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anumber</t>
   </si>
   <si>
     <t xml:space="preserve">some</t>
@@ -67,12 +70,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="16">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,16 +91,135 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -106,8 +227,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,6 +267,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -142,14 +329,91 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -158,17 +422,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,14 +450,22 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -208,60 +480,60 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -276,16 +548,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,35 +565,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>